<commit_message>
meta: update and fix examples
Fixes #54
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/line-chart-3d/line-chart-3d.xlsx
+++ b/_examples/spreadsheet/line-chart-3d/line-chart-3d.xlsx
@@ -1,83 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:sheets>
-    <x:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
-  </x:sheets>
-</x:workbook>
+<ma:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:sheets>
+    <ma:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
+  </ma:sheets>
+</ma:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="9" uniqueCount="9">
-  <x:si>
-    <x:t>Item</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Price</x:t>
-  </x:si>
-  <x:si>
-    <x:t># Sold</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 5</x:t>
-  </x:si>
-</x:sst>
+<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="9" uniqueCount="9">
+  <ma:si>
+    <ma:t>Item</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Price</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t># Sold</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Total</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 1</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 2</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 3</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 4</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 5</ma:t>
+  </ma:si>
+</ma:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:fonts count="1">
-    <x:font>
-      <x:name val="Calibri"/>
-      <x:sz val="11"/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="2">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-</x:styleSheet>
+<ma:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:fonts count="1">
+    <ma:font>
+      <ma:name val="Calibri"/>
+      <ma:sz val="11"/>
+    </ma:font>
+  </ma:fonts>
+  <ma:fills count="2">
+    <ma:fill>
+      <ma:patternFill patternType="none"/>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="gray125"/>
+    </ma:fill>
+  </ma:fills>
+  <ma:borders count="1">
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top/>
+      <ma:bottom/>
+      <ma:diagonal/>
+    </ma:border>
+  </ma:borders>
+  <ma:cellStyleXfs count="1">
+    <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </ma:cellStyleXfs>
+  <ma:cellXfs count="1">
+    <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </ma:cellXfs>
+  <ma:cellStyles count="1">
+    <ma:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </ma:cellStyles>
+</ma:styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <c:chart>
     <c:title>
       <c:tx>
@@ -255,7 +255,7 @@
         </c:spPr>
         <c:crossAx val="449512514"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
         <c:axId val="449512514"/>
@@ -336,7 +336,7 @@
       <xdr:xfrm/>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId1"/>
+          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -346,94 +346,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:dimension ref="A1"/>
-  <x:sheetData>
-    <x:row r="1">
-      <x:c t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2">
-      <x:c t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>1.23</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:f>C2*B2</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="3">
-      <x:c t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>2.46</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:f>C3*B3</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>3.69</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:f>C4*B4</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="5">
-      <x:c t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>4.92</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:f>C5*B5</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="6">
-      <x:c t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>6.15</x:v>
-      </x:c>
-      <x:c t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:f>C6*B6</x:f>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:drawing r:id="rId1"/>
-</x:worksheet>
+<ma:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:dimension ref="A1"/>
+  <ma:sheetData>
+    <ma:row r="1">
+      <ma:c r="A1" t="s">
+        <ma:v>0</ma:v>
+      </ma:c>
+      <ma:c r="B1" t="s">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="C1" t="s">
+        <ma:v>2</ma:v>
+      </ma:c>
+      <ma:c r="D1" t="s">
+        <ma:v>3</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="2">
+      <ma:c r="A2" t="s">
+        <ma:v>4</ma:v>
+      </ma:c>
+      <ma:c r="B2" t="n">
+        <ma:v>1.23</ma:v>
+      </ma:c>
+      <ma:c r="C2" t="n">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="D2" t="str">
+        <ma:f>C2*B2</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="3">
+      <ma:c r="A3" t="s">
+        <ma:v>5</ma:v>
+      </ma:c>
+      <ma:c r="B3" t="n">
+        <ma:v>2.46</ma:v>
+      </ma:c>
+      <ma:c r="C3" t="n">
+        <ma:v>2</ma:v>
+      </ma:c>
+      <ma:c r="D3" t="str">
+        <ma:f>C3*B3</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="4">
+      <ma:c r="A4" t="s">
+        <ma:v>6</ma:v>
+      </ma:c>
+      <ma:c r="B4" t="n">
+        <ma:v>3.69</ma:v>
+      </ma:c>
+      <ma:c r="C4" t="n">
+        <ma:v>3</ma:v>
+      </ma:c>
+      <ma:c r="D4" t="str">
+        <ma:f>C4*B4</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="5">
+      <ma:c r="A5" t="s">
+        <ma:v>7</ma:v>
+      </ma:c>
+      <ma:c r="B5" t="n">
+        <ma:v>4.92</ma:v>
+      </ma:c>
+      <ma:c r="C5" t="n">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="D5" t="str">
+        <ma:f>C5*B5</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="6">
+      <ma:c r="A6" t="s">
+        <ma:v>8</ma:v>
+      </ma:c>
+      <ma:c r="B6" t="n">
+        <ma:v>6.15</ma:v>
+      </ma:c>
+      <ma:c r="C6" t="n">
+        <ma:v>2</ma:v>
+      </ma:c>
+      <ma:c r="D6" t="str">
+        <ma:f>C6*B6</ma:f>
+      </ma:c>
+    </ma:row>
+  </ma:sheetData>
+  <ma:drawing r:id="rId1"/>
+</ma:worksheet>
 </file>
</xml_diff>